<commit_message>
Change the logic inside the function Get-UniqueDriveToFrom to fix logic error
Altered the function Get-UniqueDriveToFrom to fix an issue with it sometimes not combining destination drives when restoring (what was the Source drives in the file).  Also added the Write-Host to the screen to display the copying from/to message.
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BraxtonWright\Desktop\Auto Backup Script\Jobs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BraxtonWright\Desktop\Robocopy-Backup-Utility\Jobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Source</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>FileExtension</t>
+  </si>
+  <si>
+    <t>File name\Extensions seperated by a '/' for every entry</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,6 +378,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Script in a functional state
The script will now run and back up files to your system.  The only things I have to work on is the following:
1.  Have the code inside the function Start-Backup dealing with the individual files display’s its progress when it is done copying the file.
2.  Need to change the examples inside the Template (save as a csv).xlsx file because I returned to the –match operator instead of the –like when I was working on in this work session.
3.  Need to change the write-progress parameters so it will say “(Generating backup/Restoring files)” for the overall progress and “Currently (backing up/restoring): $JobName” for the job.
4.  And lastly, I need to change the function "Get-TimeRemaining" so it uses a different formula to calculate the time remaining more accurately.
All other changes are not of immediate importance, they can be implemented latter.
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Source</t>
   </si>
@@ -38,7 +38,37 @@
     <t>FileExtension</t>
   </si>
   <si>
-    <t>File name\Extensions seperated by a '/' for every entry</t>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Here are some examples all you have to do is to remove the '' around the text</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '*.txt ' will get all files that end in '.txt'</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'name* ' will get all files that start with 'name'</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '*name* ' will get all files that contains 'name'</t>
+  </si>
+  <si>
+    <t>DELETE THIS ROW WHEN YOU SAVE:  The default process is backup, so when you run a backup, it will read from the "Source" column and put it into the "Destination" column.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'name*.txt' will get all files that start with 'name' and ends in '.txt'</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  As shown by the last example you can combine them to make complex patterns such as the following</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'start * middle * end.txt' will get all files that start with 'start ', and somewhere in the middle has ' middle ', and ends with  ' end.txt'</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Using a pattern, with the * as any number of characters, you can fetch the desired files seperated by a '/' for every entry</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Need to change the examples because I had to return to the -match comparison operator and not the -like operator</t>
   </si>
 </sst>
 </file>
@@ -356,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -366,24 +396,75 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Template (save as a csv).xlsx and AuotBackup.ps1 files
Now the file Template (save as a csv).xlsx correctly explains what to do to select specific files and also change the column label from FileExtension, which is not a accurate describer, to FileMatching.  Thus the required the every instance of FileExtension to be replaced with FileMatching inside the file AutoBackup.ps1.
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -35,50 +35,58 @@
     <t>Description</t>
   </si>
   <si>
-    <t>FileExtension</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Here are some examples all you have to do is to remove the '' around the text</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '*.txt ' will get all files that end in '.txt'</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'name* ' will get all files that start with 'name'</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '*name* ' will get all files that contains 'name'</t>
-  </si>
-  <si>
     <t>DELETE THIS ROW WHEN YOU SAVE:  The default process is backup, so when you run a backup, it will read from the "Source" column and put it into the "Destination" column.</t>
   </si>
   <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'name*.txt' will get all files that start with 'name' and ends in '.txt'</t>
-  </si>
-  <si>
     <t>REMOVE\REPLACE ME WHEN YOU SAVE:  As shown by the last example you can combine them to make complex patterns such as the following</t>
   </si>
   <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'start * middle * end.txt' will get all files that start with 'start ', and somewhere in the middle has ' middle ', and ends with  ' end.txt'</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Using a pattern, with the * as any number of characters, you can fetch the desired files seperated by a '/' for every entry</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Need to change the examples because I had to return to the -match comparison operator and not the -like operator</t>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Here are some examples all you have to do is to remove the '' around the text.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Using a regex pattern, you can fetch the desired files seperated by a '/' for every pattern/entry you want to match to.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'text' will get all files that contains 'text' inside it's name.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^text' will get all files that start with 'text' inside it's name.  The ^ means at the start of the string.</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '.txt$' will get all files that end in '.txt' inside it's name.  The $ means the end of the string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^text(?:\N)*.txt$' will get all files that start with 'text' with anything between the start and the end, even nothing, and ends with '.txt' </t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^test (?:\N)*file(?:\N)* name\.txt$' will get all files that start with 'start ', and somewhere in the middle has 'file', and ends with  ' name.txt'</t>
+  </si>
+  <si>
+    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  A good place to test and learn about regex patterns can be found here</t>
+  </si>
+  <si>
+    <t>FileMatching</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,13 +109,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,14 +400,14 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -410,61 +421,64 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>11</v>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the Get-TimeRemaing so it is calculating the instantaneous time remaining intead of the average.
I have finished modifying the Get-TimeRemaing function so it is instantaneous and not the average.
This is almost a complete code, however I have not implemented the Write-Progress for single items and threading the counting of the files.
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Delete Me When Saving To CSV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Source</t>
   </si>
@@ -35,40 +36,46 @@
     <t>Description</t>
   </si>
   <si>
-    <t>DELETE THIS ROW WHEN YOU SAVE:  The default process is backup, so when you run a backup, it will read from the "Source" column and put it into the "Destination" column.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  As shown by the last example you can combine them to make complex patterns such as the following</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Here are some examples all you have to do is to remove the '' around the text.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Using a regex pattern, you can fetch the desired files seperated by a '/' for every pattern/entry you want to match to.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: 'text' will get all files that contains 'text' inside it's name.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^text' will get all files that start with 'text' inside it's name.  The ^ means at the start of the string.</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '.txt$' will get all files that end in '.txt' inside it's name.  The $ means the end of the string.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^text(?:\N)*.txt$' will get all files that start with 'text' with anything between the start and the end, even nothing, and ends with '.txt' </t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  Example: '^test (?:\N)*file(?:\N)* name\.txt$' will get all files that start with 'start ', and somewhere in the middle has 'file', and ends with  ' name.txt'</t>
-  </si>
-  <si>
-    <t>REMOVE\REPLACE ME WHEN YOU SAVE:  A good place to test and learn about regex patterns can be found here</t>
-  </si>
-  <si>
     <t>FileMatching</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>The default process is backup, so when you run a backup, it will read from the "Source" column and put it into the "Destination" column.</t>
+  </si>
+  <si>
+    <t>FileMatching Field help</t>
+  </si>
+  <si>
+    <t>Using a regex pattern, you can fetch the desired files seperated by a '/' for every pattern/entry you want to match to.</t>
+  </si>
+  <si>
+    <t>Here are some examples all you have to do is to remove the '' around the text.</t>
+  </si>
+  <si>
+    <t>Example: '.txt$' will get all files that end in '.txt' inside it's name.  The $ means the end of the string.</t>
+  </si>
+  <si>
+    <t>Example: '^text' will get all files that start with 'text' inside it's name.  The ^ means at the start of the string.</t>
+  </si>
+  <si>
+    <t>Example: 'text' will get all files that contains 'text' inside it's name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: '^text(?:\N)*.txt$' will get all files that start with 'text' with anything between the start and the end, even nothing, and ends with '.txt' </t>
+  </si>
+  <si>
+    <t>As shown by the last example you can combine them to make complex patterns such as the following</t>
+  </si>
+  <si>
+    <t>Example: '^test (?:\N)*file(?:\N)* name\.txt$' will get all files that start with 'start ', and somewhere in the middle has 'file', and ends with  ' name.txt'</t>
+  </si>
+  <si>
+    <t>A good place to learn and test regex patterns can be found here</t>
+  </si>
+  <si>
+    <t>Or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters.</t>
   </si>
 </sst>
 </file>
@@ -397,88 +404,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>13</v>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
+    <hyperlink ref="A13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed some formatting and the template file
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Source</t>
   </si>
@@ -76,6 +76,27 @@
   </si>
   <si>
     <t>Or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters.</t>
+  </si>
+  <si>
+    <t>C:\Users\BraxtonWright\Desktop\Ark files</t>
+  </si>
+  <si>
+    <t>H:\my games\Steam\Game notes\Ark files</t>
+  </si>
+  <si>
+    <t>Ark notes</t>
+  </si>
+  <si>
+    <t>C:\Users\BraxtonWright\Desktop</t>
+  </si>
+  <si>
+    <t>Satisfactory notes</t>
+  </si>
+  <si>
+    <t>H:\my games\Steam\Game notes\Satisfactory files</t>
+  </si>
+  <si>
+    <t>^Satisfactory.txt$</t>
   </si>
 </sst>
 </file>
@@ -404,9 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -422,6 +445,31 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced custom copy-item with robocopy (#9 of Todo.docx)
Now instead of using the function "Copy-ItemWithProgress" we simply use the "Robocopy" to achieve the same thing, but with a lot less code.

This set of modification also changed how you define the FileMatching field for the job csv file.  Now, instead of using Regular Expressions, now you define them using Wildcard Expressions.
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="11550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="11550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Source</t>
   </si>
@@ -45,65 +45,50 @@
     <t>The default process is backup, so when you run a backup, it will read from the "Source" column and put it into the "Destination" column.</t>
   </si>
   <si>
-    <t>FileMatching Field help</t>
-  </si>
-  <si>
-    <t>Using a regex pattern, you can fetch the desired files seperated by a '/' for every pattern/entry you want to match to.</t>
-  </si>
-  <si>
     <t>Here are some examples all you have to do is to remove the '' around the text.</t>
   </si>
   <si>
-    <t>Example: '.txt$' will get all files that end in '.txt' inside it's name.  The $ means the end of the string.</t>
-  </si>
-  <si>
-    <t>Example: '^text' will get all files that start with 'text' inside it's name.  The ^ means at the start of the string.</t>
-  </si>
-  <si>
-    <t>Example: 'text' will get all files that contains 'text' inside it's name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example: '^text(?:\N)*.txt$' will get all files that start with 'text' with anything between the start and the end, even nothing, and ends with '.txt' </t>
-  </si>
-  <si>
-    <t>As shown by the last example you can combine them to make complex patterns such as the following</t>
-  </si>
-  <si>
-    <t>Example: '^test (?:\N)*file(?:\N)* name\.txt$' will get all files that start with 'start ', and somewhere in the middle has 'file', and ends with  ' name.txt'</t>
-  </si>
-  <si>
-    <t>A good place to learn and test regex patterns can be found here</t>
-  </si>
-  <si>
     <t>Or you can leave it blank to get ALL the contents of the folder.  This is case insensitive so you don't need to worry about capital letters.</t>
   </si>
   <si>
-    <t>C:\Users\BraxtonWright\Desktop\Ark files</t>
-  </si>
-  <si>
-    <t>H:\my games\Steam\Game notes\Ark files</t>
-  </si>
-  <si>
-    <t>Ark notes</t>
-  </si>
-  <si>
-    <t>C:\Users\BraxtonWright\Desktop</t>
-  </si>
-  <si>
-    <t>Satisfactory notes</t>
-  </si>
-  <si>
-    <t>H:\my games\Steam\Game notes\Satisfactory files</t>
-  </si>
-  <si>
-    <t>^Satisfactory.txt$</t>
+    <t>Using combination of powershell wildcard characters, you can fetch the desired files seperated by a '/' for every pattern/entry you want to match to.</t>
+  </si>
+  <si>
+    <t>As shown by the last example you can combine them to make complex patterns, such as the following</t>
+  </si>
+  <si>
+    <t>Example: 'test *file* name.txt' will get all files that start with 'start ', and somewhere in the middle has 'file', and ends with  ' name.txt'</t>
+  </si>
+  <si>
+    <t>Here you can learn about all the valid wildcards you can use to configure this file</t>
+  </si>
+  <si>
+    <t>FileMatching field help</t>
+  </si>
+  <si>
+    <t>Example: '*.txt' will get all files that end with '.txt'.</t>
+  </si>
+  <si>
+    <t>Example: 'text*' will get all files that start with 'text'.</t>
+  </si>
+  <si>
+    <t>Example: '*text*' will get all files that contains 'text'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: 'text*.txt' will get all files that start with 'text' with anything number of characters after it, even nothing, and ends with '.txt' </t>
+  </si>
+  <si>
+    <t>If you define a condition inside the FileMatching field, it will not remove any extra files in the source/destination folder if they are not in the other folder.  Even if they match one of the condition(s) you defined.</t>
+  </si>
+  <si>
+    <t>But if you don't define the FileMatching field, it will remove any extra files from the source/destination if they are not in the other folder.  I.E. It will make the folders mirror images of each other.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +100,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,9 +133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -425,11 +418,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -445,31 +436,6 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -480,9 +446,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -496,65 +462,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
+      <c r="A6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
+      <c r="A7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A16" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Simpiflied the fullPathRegex variable
</commit_message>
<xml_diff>
--- a/Jobs/Template (save as a csv).xlsx
+++ b/Jobs/Template (save as a csv).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="11550" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,9 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -483,9 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>